<commit_message>
added AboutPage and AboutTest
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/openemrdata.xlsx
+++ b/src/test/resources/testdata/openemrdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidyashree.logavi\eclipse-workspace\OpenEmrApplication\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B6ABBC-663A-44C9-A50D-A243BC1611B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CA8A75-3605-4C77-94B5-4236CECD0BC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7C256982-12FB-48CE-B8A7-77E848490144}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7C256982-12FB-48CE-B8A7-77E848490144}"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
+    <sheet name="checkAboutHeaderAndVersionTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -64,6 +65,33 @@
   </si>
   <si>
     <t>john123</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>expHeader</t>
+  </si>
+  <si>
+    <t>expVersion</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>About OpenEMR</t>
+  </si>
+  <si>
+    <t>v6.0.0</t>
+  </si>
+  <si>
+    <t>accountant</t>
   </si>
 </sst>
 </file>
@@ -417,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C3CA0D-FD3A-40F1-AC0A-BE13F55ABA43}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,4 +502,70 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7990687-6326-4CAC-8EB2-872A349D5F39}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>